<commit_message>
Revision 2 - Approvalflow added
</commit_message>
<xml_diff>
--- a/topcode_db_design.xlsx
+++ b/topcode_db_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="9285" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="db_design" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>Account</t>
   </si>
@@ -66,9 +66,6 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>towername</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>tower</t>
-  </si>
-  <si>
     <t>short_desc</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>req_id</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>Technical manager</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>techmanager_user_role_id</t>
   </si>
   <si>
-    <t>accautomationowner_user_role_id</t>
-  </si>
-  <si>
     <t>primaryowner_user_role_id</t>
   </si>
   <si>
@@ -298,6 +286,63 @@
   </si>
   <si>
     <t>Solution either from new request/idea</t>
+  </si>
+  <si>
+    <t>approval_id</t>
+  </si>
+  <si>
+    <t>approval_status</t>
+  </si>
+  <si>
+    <t>approver_user_role_id</t>
+  </si>
+  <si>
+    <t>approver_comments</t>
+  </si>
+  <si>
+    <t>approval_type</t>
+  </si>
+  <si>
+    <t>Ideator</t>
+  </si>
+  <si>
+    <t>Person who posts the idea</t>
+  </si>
+  <si>
+    <t>posted_user_role_id</t>
+  </si>
+  <si>
+    <t>final_approval_id</t>
+  </si>
+  <si>
+    <t>ApprovalFlowHistory</t>
+  </si>
+  <si>
+    <t>approval_history_id</t>
+  </si>
+  <si>
+    <t>modified_user_role_id</t>
+  </si>
+  <si>
+    <t>posted_dt</t>
+  </si>
+  <si>
+    <t>modified_dt</t>
+  </si>
+  <si>
+    <t>modify_comments</t>
+  </si>
+  <si>
+    <t>type(req/idea)</t>
+  </si>
+  <si>
+    <t>request_id</t>
+  </si>
+  <si>
+    <t>acc_automation_owner_user_role_id</t>
+  </si>
+  <si>
+    <t>eng_member_role(dev/qa/business)</t>
   </si>
 </sst>
 </file>
@@ -337,7 +382,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -386,14 +431,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -405,6 +460,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +781,7 @@
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="12" width="22.5703125" customWidth="1"/>
@@ -730,343 +789,391 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="E17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="E18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row r="28" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="1"/>
+      <c r="E32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E28" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="4" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="E32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1077,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A12:B21"/>
+  <dimension ref="A12:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,15 +1206,15 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1115,55 +1222,63 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1187,10 +1302,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1329,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,15 +1337,15 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>